<commit_message>
add Assign User Garbage Collect scenario
</commit_message>
<xml_diff>
--- a/Automation-Template/qa-automation-template-master/data/locatorsRepository.xlsx
+++ b/Automation-Template/qa-automation-template-master/data/locatorsRepository.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDUCATION\SLIIT\4 Year\Y4 S2\SQA\TrashMate-Automation\Automation-Template\qa-automation-template-master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Y4\SQA\Assignment\TrashMate-Automation\Automation-Template\qa-automation-template-master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB570C3-CCFA-4FF3-8822-C93C133DFB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55811265-35FB-4F1A-B1B9-10C550800FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6EC30635-A69F-42C4-9C00-4643C4E984B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EC30635-A69F-42C4-9C00-4643C4E984B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Web" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>ElementID</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>Assigned_User_Button</t>
+  </si>
+  <si>
+    <t>//a[normalize-space()='Assigned Users']</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='Collect Garbage']</t>
+  </si>
+  <si>
+    <t>Collect_Garbage_Button</t>
+  </si>
+  <si>
+    <t>//select[@class='form-select']</t>
+  </si>
+  <si>
+    <t>Waste_Type_Selector</t>
   </si>
 </sst>
 </file>
@@ -549,17 +567,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97E25B-5CF4-4671-ADCD-82227B0F14A0}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="120.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="120.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -690,6 +708,39 @@
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>